<commit_message>
feat : Lombok에 관하여
</commit_message>
<xml_diff>
--- a/민영/220105_A프로젝트_기능명세서_김민영.xlsx
+++ b/민영/220105_A프로젝트_기능명세서_김민영.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dw-012\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dw-014\Desktop\김민영\민영\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,180 +27,182 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>A프로젝트 기능명세서</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>중분류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>소분류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>개발 소요일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>개발 예정일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>개발일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>우선순위</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>비고</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이발예약</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이발병 스케줄 관리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스케줄 등록 - 일자별 예약시간</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 07일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>中</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스케줄 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스케줄 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예약 승인</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예약현황 PDF 파일로 출력</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그관리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이발 예약</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이발 예약 날짜 변경</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이발 예약 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 05일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 05일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 09일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 12일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>01월 14일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>01월 10일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>01월 17일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>上</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>下</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>中</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>上</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>下</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>中</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>下</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>간부 예약부터 작업해야함.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>병사,간부 이발 예약</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>대분류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>총 개발 소요일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 메일함 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 기능</t>
+  </si>
+  <si>
+    <t>메일 목록 열람 기능</t>
+  </si>
+  <si>
+    <t>최신 메일 목록 열람 기능</t>
+  </si>
+  <si>
+    <t>특정 메일 삭제 기능</t>
+  </si>
+  <si>
+    <t>선택한 메일 작성 기능</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선택</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기능</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차 스프린트 때 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -222,8 +224,21 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,12 +254,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +287,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,13 +297,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,7 +595,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C17:C18"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -597,15 +609,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -630,182 +642,156 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="1" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="1" t="s">
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="1" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <f>SUM(D4:D12)</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +802,7 @@
     <mergeCell ref="A4:A12"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>